<commit_message>
correction of mistake in demographic data
</commit_message>
<xml_diff>
--- a/data/PET1_adult_pilot_demo_data.xlsx
+++ b/data/PET1_adult_pilot_demo_data.xlsx
@@ -1,28 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christoph Voelter\Documents\_git\PET1_adult_pilot\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{066B39D6-C52A-43CF-A928-963CA395CF7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="demo_data" sheetId="1" r:id="rId1"/>
-    <sheet name="variables" sheetId="2" r:id="rId2"/>
-    <sheet name="instruction" sheetId="3" r:id="rId3"/>
+    <sheet name="demo_data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="variables" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="instruction" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
   <si>
     <t>subject</t>
   </si>
@@ -117,7 +110,7 @@
     <t>21.12.1981</t>
   </si>
   <si>
-    <t>the video was sometimes really slow or didnt skip to the next sequence</t>
+    <t xml:space="preserve">the video was sometimes really slow or didnt skip to the next sequence</t>
   </si>
   <si>
     <t>subj.07</t>
@@ -171,7 +164,7 @@
     <t xml:space="preserve">trägt manchmal eine brille, braucht diese aber nicht für Bildschirme </t>
   </si>
   <si>
-    <t>DROP? hat permanent make-up (liedstrich in schwarz)</t>
+    <t xml:space="preserve">DROP? hat permanent make-up (liedstrich in schwarz)</t>
   </si>
   <si>
     <t>subj.13</t>
@@ -201,7 +194,7 @@
     <t>20.03.1973</t>
   </si>
   <si>
-    <t>Teilnehmerin hat mehrfach während des Videos genießt oder sich die Nase gekratzt</t>
+    <t xml:space="preserve">Teilnehmerin hat mehrfach während des Videos genießt oder sich die Nase gekratzt</t>
   </si>
   <si>
     <t>subj.17</t>
@@ -252,7 +245,7 @@
     <t>17.01.1970</t>
   </si>
   <si>
-    <t>Teilnehmerin trägt eine Lesebrille, hatte diese während der Testung aber nicht auf.</t>
+    <t xml:space="preserve">Teilnehmerin trägt eine Lesebrille, hatte diese während der Testung aber nicht auf.</t>
   </si>
   <si>
     <t>subj.24</t>
@@ -345,7 +338,7 @@
     <t>02.06.1997</t>
   </si>
   <si>
-    <t>Haben ca 6 mal C&amp;V gemacht, die Werte blieben jedoch schlecht, egal was ich veränderte. Er meinte auch, dass er sich durch sein ADHS sehr schwer auf die Aufgaben konzentrieren konnte.</t>
+    <t xml:space="preserve">Haben ca 6 mal C&amp;V gemacht, die Werte blieben jedoch schlecht, egal was ich veränderte. Er meinte auch, dass er sich durch sein ADHS sehr schwer auf die Aufgaben konzentrieren konnte.</t>
   </si>
   <si>
     <t>subj.36</t>
@@ -387,7 +380,7 @@
     <t>18.10.1986</t>
   </si>
   <si>
-    <t>Kind war im Raum mit uns, aber leise und hat gemalt.</t>
+    <t xml:space="preserve">Kind war im Raum mit uns, aber leise und hat gemalt.</t>
   </si>
   <si>
     <t>24.09.2024</t>
@@ -399,7 +392,7 @@
     <t>Brille</t>
   </si>
   <si>
-    <t>Ist kurzsichtig, braucht seine Brille nicht Für Bildschirme.</t>
+    <t xml:space="preserve">Ist kurzsichtig, braucht seine Brille nicht Für Bildschirme.</t>
   </si>
   <si>
     <t>25.09.2024</t>
@@ -414,115 +407,112 @@
     <t>definition</t>
   </si>
   <si>
-    <t>subject ID chosen in ExperimentBuilder dropdown menu, subj.01 - subj.40</t>
-  </si>
-  <si>
-    <t>child lab data base ID</t>
-  </si>
-  <si>
-    <t>date of test, dd/mm/yyyy</t>
-  </si>
-  <si>
-    <t>birthday, dd/mm/yyyy</t>
-  </si>
-  <si>
-    <t>gender: m, f, d</t>
+    <t xml:space="preserve">subject ID chosen in ExperimentBuilder dropdown menu, subj.01 - subj.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">child lab data base ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date of test, dd/mm/yyyy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birthday, dd/mm/yyyy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender: m, f, d</t>
   </si>
   <si>
     <t>average_validation_value</t>
   </si>
   <si>
-    <t>at the end of the validation the average validation value is shown on the host PC screen</t>
+    <t xml:space="preserve">at the end of the validation the average validation value is shown on the host PC screen</t>
   </si>
   <si>
     <t>maximal_validation_value</t>
   </si>
   <si>
-    <t>at the end of the validation all validation values are shown on the host PC screen, enter the largest value</t>
-  </si>
-  <si>
-    <t>does the participant wear eyewear: no, glasses, contact_lenses</t>
-  </si>
-  <si>
-    <t>free text field</t>
-  </si>
-  <si>
-    <t>Eye-tracker controls (Host PC keyboard)</t>
+    <t xml:space="preserve">at the end of the validation all validation values are shown on the host PC screen, enter the largest value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">does the participant wear eyewear: no, glasses, contact_lenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free text field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eye-tracker controls (Host PC keyboard)</t>
   </si>
   <si>
     <t>c</t>
   </si>
   <si>
-    <t>start calibration</t>
+    <t xml:space="preserve">start calibration</t>
   </si>
   <si>
     <t>v</t>
   </si>
   <si>
-    <t>start validation</t>
+    <t xml:space="preserve">start validation</t>
   </si>
   <si>
     <t>o</t>
   </si>
   <si>
-    <t>after accepting validation via a mouse click, start data collection</t>
+    <t xml:space="preserve">after accepting validation via a mouse click, start data collection</t>
   </si>
   <si>
     <t>s</t>
   </si>
   <si>
-    <t>skip fixation trigger (should not be used during data collection)</t>
+    <t xml:space="preserve">skip fixation trigger (should not be used during data collection)</t>
   </si>
   <si>
     <t>F6</t>
   </si>
   <si>
-    <t>start another calibration at the beginning of the second block or if the eyetracker does not recognise the eye anymore during the fixation trigger</t>
-  </si>
-  <si>
-    <t>Vielen Dank, dass Sie an dieser Eye-Tracking-Studie teilnehmen. Wir beginnen mit einem Kalibrierungsprozess. Bitte schauen Sie so genau wie möglich auf die auf dem Bildschirm gezeigten Punkte.</t>
-  </si>
-  <si>
-    <t>Sie werden nun eine Reihe von kurzen Videos sehen. Bitte schauen Sie sich die Videos einfach an, wie Sie es normalerweise tun würden.</t>
-  </si>
-  <si>
-    <t>participant_id</t>
+    <t xml:space="preserve">start another calibration at the beginning of the second block or if the eyetracker does not recognise the eye anymore during the fixation trigger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vielen Dank, dass Sie an dieser Eye-Tracking-Studie teilnehmen. Wir beginnen mit einem Kalibrierungsprozess. Bitte schauen Sie so genau wie möglich auf die auf dem Bildschirm gezeigten Punkte.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sie werden nun eine Reihe von kurzen Videos sehen. Bitte schauen Sie sich die Videos einfach an, wie Sie es normalerweise tun würden.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Carlito"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <name val="Carlito"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color rgb="FF172B4D"/>
       <name val="Segoe UI"/>
     </font>
@@ -549,80 +539,84 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="23">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -630,15 +624,295 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -841,37 +1115,35 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A21" zoomScale="100" workbookViewId="0">
+      <selection activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="13.73046875" customWidth="1"/>
-    <col min="3" max="3" width="13.1328125" customWidth="1"/>
-    <col min="4" max="4" width="13.265625" customWidth="1"/>
-    <col min="6" max="6" width="30.3984375" customWidth="1"/>
-    <col min="7" max="7" width="29.59765625" customWidth="1"/>
-    <col min="8" max="8" width="28.265625" customWidth="1"/>
-    <col min="9" max="9" width="29.59765625" customWidth="1"/>
-    <col min="10" max="10" width="12.265625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="65.1328125" customWidth="1"/>
+    <col customWidth="1" min="2" max="2" width="13.765625"/>
+    <col customWidth="1" min="3" max="3" width="13.140625"/>
+    <col customWidth="1" min="4" max="4" width="13.28125"/>
+    <col customWidth="1" min="6" max="6" width="30.421875"/>
+    <col customWidth="1" min="7" max="7" width="29.57421875"/>
+    <col customWidth="1" min="8" max="8" width="28.28125"/>
+    <col customWidth="1" min="9" max="9" width="29.57421875"/>
+    <col customWidth="1" min="10" max="10" style="1" width="12.28125"/>
+    <col customWidth="1" min="11" max="11" width="65.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -901,7 +1173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" ht="16.5">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -921,13 +1193,13 @@
         <v>0.19</v>
       </c>
       <c r="G2" s="4">
-        <v>0.24</v>
+        <v>0.23999999999999999</v>
       </c>
       <c r="H2" s="4">
-        <v>0.34</v>
+        <v>0.34000000000000002</v>
       </c>
       <c r="I2" s="4">
-        <v>0.67</v>
+        <v>0.67000000000000004</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>15</v>
@@ -936,7 +1208,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" ht="16.5">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -953,16 +1225,16 @@
         <v>19</v>
       </c>
       <c r="F3" s="4">
-        <v>0.34</v>
+        <v>0.34000000000000002</v>
       </c>
       <c r="G3" s="4">
         <v>0.38</v>
       </c>
       <c r="H3" s="4">
-        <v>0.64</v>
+        <v>0.64000000000000001</v>
       </c>
       <c r="I3" s="4">
-        <v>0.6</v>
+        <v>0.59999999999999998</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>15</v>
@@ -971,7 +1243,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" ht="16.5">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -994,17 +1266,17 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="H4" s="8">
-        <v>0.49</v>
+        <v>0.48999999999999999</v>
       </c>
       <c r="I4" s="8">
-        <v>0.27</v>
+        <v>0.27000000000000002</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" ht="16.5">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1027,17 +1299,17 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="H5" s="8">
-        <v>0.52</v>
+        <v>0.52000000000000002</v>
       </c>
       <c r="I5" s="8">
-        <v>1.67</v>
+        <v>1.6699999999999999</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>15</v>
       </c>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" ht="16.5">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1057,20 +1329,20 @@
         <v>0.62</v>
       </c>
       <c r="G6" s="8">
-        <v>0.48</v>
+        <v>0.47999999999999998</v>
       </c>
       <c r="H6" s="8">
-        <v>1.9</v>
+        <v>1.8999999999999999</v>
       </c>
       <c r="I6" s="8">
-        <v>1.94</v>
+        <v>1.9399999999999999</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>15</v>
       </c>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" ht="16.5">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1087,13 +1359,13 @@
         <v>19</v>
       </c>
       <c r="F7" s="8">
-        <v>0.4</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="G7" s="8">
-        <v>0.39</v>
+        <v>0.39000000000000001</v>
       </c>
       <c r="H7" s="8">
-        <v>0.72</v>
+        <v>0.71999999999999997</v>
       </c>
       <c r="I7" s="8">
         <v>0.63</v>
@@ -1105,7 +1377,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" ht="16.5">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1125,13 +1397,13 @@
         <v>0.37</v>
       </c>
       <c r="G8" s="8">
-        <v>0.23</v>
+        <v>0.23000000000000001</v>
       </c>
       <c r="H8" s="8">
         <v>0.44</v>
       </c>
       <c r="I8" s="8">
-        <v>0.7</v>
+        <v>0.69999999999999996</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>15</v>
@@ -1140,7 +1412,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" ht="16.5">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1157,7 +1429,7 @@
         <v>19</v>
       </c>
       <c r="F9" s="8">
-        <v>0.18</v>
+        <v>0.17999999999999999</v>
       </c>
       <c r="G9" s="8">
         <v>0.19</v>
@@ -1166,7 +1438,7 @@
         <v>0.63</v>
       </c>
       <c r="I9" s="8">
-        <v>0.52</v>
+        <v>0.52000000000000002</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>15</v>
@@ -1175,7 +1447,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1192,23 +1464,23 @@
         <v>14</v>
       </c>
       <c r="F10" s="8">
-        <v>0.36</v>
+        <v>0.35999999999999999</v>
       </c>
       <c r="G10" s="8">
-        <v>0.26</v>
+        <v>0.26000000000000001</v>
       </c>
       <c r="H10" s="8">
-        <v>1.59</v>
+        <v>1.5900000000000001</v>
       </c>
       <c r="I10" s="8">
-        <v>0.48</v>
+        <v>0.47999999999999998</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1241,7 +1513,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1258,10 +1530,10 @@
         <v>14</v>
       </c>
       <c r="F12">
-        <v>0.49</v>
+        <v>0.48999999999999999</v>
       </c>
       <c r="G12">
-        <v>0.3</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="H12">
         <v>0.63</v>
@@ -1274,7 +1546,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" ht="85.5">
+    <row r="13" ht="85.5">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1291,10 +1563,10 @@
         <v>14</v>
       </c>
       <c r="F13">
-        <v>0.61</v>
+        <v>0.60999999999999999</v>
       </c>
       <c r="G13">
-        <v>0.4</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="H13">
         <v>1.03</v>
@@ -1309,7 +1581,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1326,10 +1598,10 @@
         <v>14</v>
       </c>
       <c r="F14">
-        <v>0.21</v>
+        <v>0.20999999999999999</v>
       </c>
       <c r="G14">
-        <v>0.24</v>
+        <v>0.23999999999999999</v>
       </c>
       <c r="H14">
         <v>0.28000000000000003</v>
@@ -1341,7 +1613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1358,22 +1630,22 @@
         <v>19</v>
       </c>
       <c r="F15">
-        <v>0.49</v>
+        <v>0.48999999999999999</v>
       </c>
       <c r="G15">
         <v>0.28000000000000003</v>
       </c>
       <c r="H15">
-        <v>0.98</v>
+        <v>0.97999999999999998</v>
       </c>
       <c r="I15">
-        <v>0.77</v>
+        <v>0.77000000000000002</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1390,22 +1662,22 @@
         <v>19</v>
       </c>
       <c r="F16">
-        <v>0.3</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="G16">
-        <v>0.24</v>
+        <v>0.23999999999999999</v>
       </c>
       <c r="H16">
-        <v>0.79</v>
+        <v>0.79000000000000004</v>
       </c>
       <c r="I16">
-        <v>0.47</v>
+        <v>0.46999999999999997</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="28.5">
+    <row r="17" ht="28.5">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1422,16 +1694,16 @@
         <v>14</v>
       </c>
       <c r="F17">
-        <v>0.23</v>
+        <v>0.23000000000000001</v>
       </c>
       <c r="G17">
-        <v>0.23</v>
+        <v>0.23000000000000001</v>
       </c>
       <c r="H17">
         <v>0.38</v>
       </c>
       <c r="I17">
-        <v>0.46</v>
+        <v>0.46000000000000002</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>15</v>
@@ -1440,7 +1712,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1457,10 +1729,10 @@
         <v>19</v>
       </c>
       <c r="F18">
-        <v>0.47</v>
+        <v>0.46999999999999997</v>
       </c>
       <c r="G18">
-        <v>0.4</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="H18">
         <v>0.63</v>
@@ -1472,7 +1744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -1489,7 +1761,7 @@
         <v>19</v>
       </c>
       <c r="F19">
-        <v>0.26</v>
+        <v>0.26000000000000001</v>
       </c>
       <c r="G19">
         <v>0.28999999999999998</v>
@@ -1504,7 +1776,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -1521,13 +1793,13 @@
         <v>14</v>
       </c>
       <c r="F20">
-        <v>0.35</v>
+        <v>0.34999999999999998</v>
       </c>
       <c r="G20">
-        <v>0.17</v>
+        <v>0.17000000000000001</v>
       </c>
       <c r="H20">
-        <v>0.78</v>
+        <v>0.78000000000000003</v>
       </c>
       <c r="I20">
         <v>0.55000000000000004</v>
@@ -1536,7 +1808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1553,13 +1825,13 @@
         <v>14</v>
       </c>
       <c r="F21">
-        <v>0.45</v>
+        <v>0.45000000000000001</v>
       </c>
       <c r="G21">
-        <v>0.35</v>
+        <v>0.34999999999999998</v>
       </c>
       <c r="H21">
-        <v>0.78</v>
+        <v>0.78000000000000003</v>
       </c>
       <c r="I21">
         <v>0.57999999999999996</v>
@@ -1568,7 +1840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1588,19 +1860,19 @@
         <v>0.22</v>
       </c>
       <c r="G22">
-        <v>0.17</v>
+        <v>0.17000000000000001</v>
       </c>
       <c r="H22">
         <v>0.28999999999999998</v>
       </c>
       <c r="I22">
-        <v>0.41</v>
+        <v>0.40999999999999998</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -1617,22 +1889,22 @@
         <v>14</v>
       </c>
       <c r="F23">
-        <v>0.24</v>
+        <v>0.23999999999999999</v>
       </c>
       <c r="G23">
-        <v>0.2</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="H23">
-        <v>0.67</v>
+        <v>0.67000000000000004</v>
       </c>
       <c r="I23">
-        <v>0.34</v>
+        <v>0.34000000000000002</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="28.5">
+    <row r="24" ht="28.5">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -1649,16 +1921,16 @@
         <v>14</v>
       </c>
       <c r="F24">
-        <v>0.24</v>
+        <v>0.23999999999999999</v>
       </c>
       <c r="G24">
         <v>0.28000000000000003</v>
       </c>
       <c r="H24">
-        <v>0.76</v>
+        <v>0.76000000000000001</v>
       </c>
       <c r="I24">
-        <v>0.83</v>
+        <v>0.82999999999999996</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>15</v>
@@ -1667,7 +1939,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -1690,7 +1962,7 @@
         <v>0.16</v>
       </c>
       <c r="H25">
-        <v>0.49</v>
+        <v>0.48999999999999999</v>
       </c>
       <c r="I25">
         <v>0.31</v>
@@ -1699,7 +1971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -1716,10 +1988,10 @@
         <v>14</v>
       </c>
       <c r="F26">
-        <v>0.21</v>
+        <v>0.20999999999999999</v>
       </c>
       <c r="G26">
-        <v>0.33</v>
+        <v>0.33000000000000002</v>
       </c>
       <c r="H26">
         <v>0.56000000000000005</v>
@@ -1731,7 +2003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -1748,10 +2020,10 @@
         <v>19</v>
       </c>
       <c r="F27">
-        <v>0.32</v>
+        <v>0.32000000000000001</v>
       </c>
       <c r="G27">
-        <v>0.27</v>
+        <v>0.27000000000000002</v>
       </c>
       <c r="H27">
         <v>1.27</v>
@@ -1763,7 +2035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -1780,13 +2052,13 @@
         <v>19</v>
       </c>
       <c r="F28">
-        <v>0.59</v>
+        <v>0.58999999999999997</v>
       </c>
       <c r="G28">
-        <v>0.26</v>
+        <v>0.26000000000000001</v>
       </c>
       <c r="H28">
-        <v>1.57</v>
+        <v>1.5700000000000001</v>
       </c>
       <c r="I28">
         <v>0.56999999999999995</v>
@@ -1795,7 +2067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29">
       <c r="A29" t="s">
         <v>88</v>
       </c>
@@ -1812,13 +2084,13 @@
         <v>14</v>
       </c>
       <c r="F29">
-        <v>0.42</v>
+        <v>0.41999999999999998</v>
       </c>
       <c r="G29">
-        <v>0.41</v>
+        <v>0.40999999999999998</v>
       </c>
       <c r="H29">
-        <v>0.72</v>
+        <v>0.71999999999999997</v>
       </c>
       <c r="I29">
         <v>0.57999999999999996</v>
@@ -1827,7 +2099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30">
       <c r="A30" t="s">
         <v>90</v>
       </c>
@@ -1847,19 +2119,19 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G30">
-        <v>0.26</v>
+        <v>0.26000000000000001</v>
       </c>
       <c r="H30">
-        <v>0.8</v>
+        <v>0.80000000000000004</v>
       </c>
       <c r="I30">
-        <v>0.61</v>
+        <v>0.60999999999999999</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -1879,7 +2151,7 @@
         <v>0.25</v>
       </c>
       <c r="G31">
-        <v>0.39</v>
+        <v>0.39000000000000001</v>
       </c>
       <c r="H31">
         <v>0.63</v>
@@ -1891,7 +2163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32">
       <c r="A32" t="s">
         <v>95</v>
       </c>
@@ -1908,22 +2180,22 @@
         <v>19</v>
       </c>
       <c r="F32">
-        <v>0.4</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="G32">
-        <v>0.2</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="H32">
         <v>1.49</v>
       </c>
       <c r="I32">
-        <v>0.27</v>
+        <v>0.27000000000000002</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -1940,10 +2212,10 @@
         <v>14</v>
       </c>
       <c r="F33" s="8">
-        <v>0.32</v>
+        <v>0.32000000000000001</v>
       </c>
       <c r="G33" s="8">
-        <v>0.2</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="H33" s="8">
         <v>0.38</v>
@@ -1955,7 +2227,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -1972,13 +2244,13 @@
         <v>14</v>
       </c>
       <c r="F34" s="8">
-        <v>0.33</v>
+        <v>0.33000000000000002</v>
       </c>
       <c r="G34" s="8">
         <v>0.44</v>
       </c>
       <c r="H34" s="8">
-        <v>0.77</v>
+        <v>0.77000000000000002</v>
       </c>
       <c r="I34" s="8">
         <v>0.5</v>
@@ -1987,7 +2259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -2010,16 +2282,16 @@
         <v>0.38</v>
       </c>
       <c r="H35" s="8">
-        <v>0.84</v>
+        <v>0.83999999999999997</v>
       </c>
       <c r="I35" s="8">
-        <v>0.77</v>
+        <v>0.77000000000000002</v>
       </c>
       <c r="J35" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="42.75">
+    <row r="36" ht="42.75">
       <c r="A36" s="17" t="s">
         <v>104</v>
       </c>
@@ -2036,10 +2308,10 @@
         <v>19</v>
       </c>
       <c r="F36" s="17">
-        <v>0.72</v>
+        <v>0.71999999999999997</v>
       </c>
       <c r="G36" s="17">
-        <v>0.51</v>
+        <v>0.51000000000000001</v>
       </c>
       <c r="H36" s="17">
         <v>4.04</v>
@@ -2054,7 +2326,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -2071,10 +2343,10 @@
         <v>19</v>
       </c>
       <c r="F37">
-        <v>0.23</v>
+        <v>0.23000000000000001</v>
       </c>
       <c r="G37">
-        <v>0.2</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="H37">
         <v>0.63</v>
@@ -2086,12 +2358,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38">
       <c r="A38" t="s">
         <v>110</v>
       </c>
       <c r="B38">
-        <v>282654</v>
+        <v>282653</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>105</v>
@@ -2109,21 +2381,21 @@
         <v>0.25</v>
       </c>
       <c r="H38">
-        <v>0.43</v>
+        <v>0.42999999999999999</v>
       </c>
       <c r="I38">
-        <v>0.48</v>
+        <v>0.47999999999999998</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39">
       <c r="A39" t="s">
         <v>112</v>
       </c>
       <c r="B39" s="2">
-        <v>285126</v>
+        <v>284126</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>113</v>
@@ -2135,22 +2407,22 @@
         <v>19</v>
       </c>
       <c r="F39">
-        <v>0.4</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="G39">
-        <v>0.24</v>
+        <v>0.23999999999999999</v>
       </c>
       <c r="H39">
-        <v>0.92</v>
+        <v>0.92000000000000004</v>
       </c>
       <c r="I39">
-        <v>0.46</v>
+        <v>0.46000000000000002</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40">
       <c r="A40" t="s">
         <v>115</v>
       </c>
@@ -2173,16 +2445,16 @@
         <v>0.19</v>
       </c>
       <c r="H40">
-        <v>0.41</v>
+        <v>0.40999999999999998</v>
       </c>
       <c r="I40">
-        <v>0.36</v>
+        <v>0.35999999999999999</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41">
       <c r="A41" t="s">
         <v>117</v>
       </c>
@@ -2199,7 +2471,7 @@
         <v>19</v>
       </c>
       <c r="F41">
-        <v>0.21</v>
+        <v>0.20999999999999999</v>
       </c>
       <c r="G41">
         <v>0.22</v>
@@ -2208,13 +2480,13 @@
         <v>0.44</v>
       </c>
       <c r="I41">
-        <v>0.42</v>
+        <v>0.41999999999999998</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" ht="14.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -2234,13 +2506,13 @@
         <v>0.25</v>
       </c>
       <c r="G42">
-        <v>0.41</v>
+        <v>0.40999999999999998</v>
       </c>
       <c r="H42">
         <v>0.75</v>
       </c>
       <c r="I42">
-        <v>0.76</v>
+        <v>0.76000000000000001</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>15</v>
@@ -2249,7 +2521,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" ht="14.25">
       <c r="A43" s="17" t="s">
         <v>17</v>
       </c>
@@ -2269,13 +2541,13 @@
         <v>0.25</v>
       </c>
       <c r="G43" s="17">
-        <v>0.34</v>
+        <v>0.34000000000000002</v>
       </c>
       <c r="H43" s="17">
-        <v>0.42</v>
+        <v>0.41999999999999998</v>
       </c>
       <c r="I43" s="17">
-        <v>0.6</v>
+        <v>0.59999999999999998</v>
       </c>
       <c r="J43" s="20" t="s">
         <v>124</v>
@@ -2284,14 +2556,14 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" ht="14.25">
       <c r="A44" t="s">
         <v>28</v>
       </c>
       <c r="B44" s="2">
         <v>261242</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C44" s="11" t="s">
         <v>126</v>
       </c>
       <c r="D44" s="11" t="s">
@@ -2304,38 +2576,39 @@
         <v>0.38</v>
       </c>
       <c r="G44">
-        <v>0.3</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="H44">
-        <v>0.64</v>
+        <v>0.64000000000000001</v>
       </c>
       <c r="I44">
-        <v>0.45</v>
+        <v>0.45000000000000001</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="27.3984375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="27.3828125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -2343,7 +2616,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2351,7 +2624,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2359,7 +2632,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2367,7 +2640,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2375,7 +2648,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2383,7 +2656,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -2391,7 +2664,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8">
       <c r="A8" t="s">
         <v>137</v>
       </c>
@@ -2399,7 +2672,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2407,7 +2680,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2415,12 +2688,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14">
       <c r="A14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -2428,7 +2701,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16">
       <c r="A16" t="s">
         <v>144</v>
       </c>
@@ -2436,7 +2709,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17">
       <c r="A17" t="s">
         <v>146</v>
       </c>
@@ -2444,7 +2717,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18">
       <c r="A18" t="s">
         <v>148</v>
       </c>
@@ -2452,7 +2725,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19">
       <c r="A19" t="s">
         <v>150</v>
       </c>
@@ -2461,39 +2734,42 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="88.1328125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="88.15234375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="15" customFormat="1" ht="83.65" customHeight="1">
-      <c r="A1" s="23" t="s">
+    <row r="1" s="15" customFormat="1" ht="83.599999999999994" customHeight="1">
+      <c r="A1" s="22" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="15" customFormat="1" ht="83.65" customHeight="1">
-      <c r="A2" s="23" t="s">
+    <row r="2" s="15" customFormat="1" ht="83.599999999999994" customHeight="1">
+      <c r="A2" s="22" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="15" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A3" s="23"/>
+    <row r="3" s="15" customFormat="1" ht="18.899999999999999" customHeight="1">
+      <c r="A3" s="22"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>